<commit_message>
user authentication added and design improved
</commit_message>
<xml_diff>
--- a/Assetes & Custody.xlsx
+++ b/Assetes & Custody.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F198"/>
+  <dimension ref="A1:F199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6426,6 +6426,36 @@
         </is>
       </c>
     </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>Mohammed Abu Issa</t>
+        </is>
+      </c>
+      <c r="B199" t="n">
+        <v>1505</v>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>Sales</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>ASUS ExpertBook Core i5-10210, Ram 16GB, HDD 512GB, Widows 10 Pro</t>
+        </is>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>M1NXCV18Y472045</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>